<commit_message>
notiondan bişeyler ve cost anal
</commit_message>
<xml_diff>
--- a/ Cost Analysis EED3009.xlsx
+++ b/ Cost Analysis EED3009.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elifsezinozyigit/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\_School\2022-2023\EED 3009\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A699286-C1D5-E047-B1DA-15B90B015296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6212E1D4-3B9E-4596-861D-C4EE05629B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20000" yWindow="9660" windowWidth="28040" windowHeight="17440" xr2:uid="{2687C84E-284E-174B-A7EA-0A604D782B13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2687C84E-284E-174B-A7EA-0A604D782B13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Type</t>
   </si>
@@ -133,10 +133,16 @@
     <t>15 ₺</t>
   </si>
   <si>
-    <t>113.05 ₺</t>
-  </si>
-  <si>
     <t>HCSR04</t>
+  </si>
+  <si>
+    <t>Logic Buffer/Scmt. Trig.</t>
+  </si>
+  <si>
+    <t>74HC14</t>
+  </si>
+  <si>
+    <t>116.35 ₺</t>
   </si>
 </sst>
 </file>
@@ -392,13 +398,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4983329-DF81-084C-AF8A-A0A49DFF7A8D}" name="Table1" displayName="Table1" ref="B2:E14" totalsRowCount="1" headerRowDxfId="6" dataDxfId="7">
-  <autoFilter ref="B2:E13" xr:uid="{C4983329-DF81-084C-AF8A-A0A49DFF7A8D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4983329-DF81-084C-AF8A-A0A49DFF7A8D}" name="Table1" displayName="Table1" ref="B2:E15" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:E14" xr:uid="{C4983329-DF81-084C-AF8A-A0A49DFF7A8D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9CF58396-6502-784F-B90C-34BA98D44733}" name="Type" dataDxfId="9" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2283472B-7306-C341-AEE5-FF7E2106AE7D}" name="Model" dataDxfId="5" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{99115B7A-E96B-3D47-A64D-4705AC2BCE9A}" name="Number" dataDxfId="4" totalsRowDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{6BAB593A-F123-4E4C-81E4-57BCE10972C1}" name="Total Cost" totalsRowLabel="113.05 ₺" dataDxfId="8" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9CF58396-6502-784F-B90C-34BA98D44733}" name="Type" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{2283472B-7306-C341-AEE5-FF7E2106AE7D}" name="Model" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{99115B7A-E96B-3D47-A64D-4705AC2BCE9A}" name="Number" dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{6BAB593A-F123-4E4C-81E4-57BCE10972C1}" name="Total Cost" totalsRowLabel="116.35 ₺" dataDxfId="4" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -701,21 +707,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9096947-B2FE-784F-A795-6964F72C54B1}">
-  <dimension ref="B2:E14"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -729,12 +735,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -743,7 +749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -757,65 +763,65 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
@@ -827,64 +833,78 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>